<commit_message>
update datatest - 288 scope, 1212 maytronics,
</commit_message>
<xml_diff>
--- a/fin_scrapy/maya/data/datatest.xlsx
+++ b/fin_scrapy/maya/data/datatest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naama\PycharmProjects\finance_book\fin_scrapy\maya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFFAF13D-F920-4F8E-A31D-837545E939AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6900132C-984A-4A4E-BDF7-DB91863B6DBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9F26097-3032-4D88-B237-30A8AA0DDC42}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>#</t>
   </si>
@@ -114,6 +114,21 @@
   </si>
   <si>
     <t>68_2016</t>
+  </si>
+  <si>
+    <t>cfpage</t>
+  </si>
+  <si>
+    <t>KPMG</t>
+  </si>
+  <si>
+    <t>1054_2016</t>
+  </si>
+  <si>
+    <t>1054_2018</t>
+  </si>
+  <si>
+    <t>מתוך</t>
   </si>
 </sst>
 </file>
@@ -173,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -479,13 +494,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -562,15 +628,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,14 +670,24 @@
     <xf numFmtId="17" fontId="2" fillId="2" borderId="18" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - הדגשה5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - הדגשה6" xfId="2" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -908,86 +999,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1DC888-ECA5-4870-9572-058C60F3D853}">
-  <dimension ref="A1:AR11"/>
+  <dimension ref="A1:AZ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="31" max="31" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="9.33203125" customWidth="1"/>
+    <col min="24" max="24" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.75" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="28">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="30">
         <v>2015</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28">
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="30">
         <v>2016</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="28">
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="30">
         <v>2017</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="28">
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="30">
         <v>2018</v>
       </c>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="32" t="s">
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="29" t="s">
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="29" t="s">
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="30"/>
-      <c r="AK1" s="30"/>
-      <c r="AL1" s="30"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="29" t="s">
+      <c r="AP1" s="35"/>
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="30"/>
-      <c r="AR1" s="31"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="36"/>
     </row>
-    <row r="2" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
@@ -1010,70 +1115,72 @@
       <c r="H2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="17"/>
+      <c r="L2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="M2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="17"/>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="17"/>
+      <c r="R2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="S2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="U2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="V2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="17"/>
-      <c r="U2" s="14" t="s">
+      <c r="W2" s="17"/>
+      <c r="X2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="Y2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="15" t="s">
+      <c r="Z2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="AA2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="14" t="s">
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="15" t="s">
+      <c r="AE2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="15" t="s">
+      <c r="AF2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG2" s="15" t="s">
-        <v>16</v>
+      <c r="AG2" s="26" t="s">
+        <v>28</v>
       </c>
       <c r="AH2" s="16" t="s">
         <v>13</v>
@@ -1088,24 +1195,46 @@
       <c r="AL2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AM2" s="16" t="s">
+      <c r="AM2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="AN2" s="17"/>
-      <c r="AO2" s="14" t="s">
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AP2" s="15" t="s">
+      <c r="AQ2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AQ2" s="15" t="s">
+      <c r="AR2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AR2" s="16" t="s">
+      <c r="AS2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT2" s="16" t="s">
         <v>13</v>
       </c>
+      <c r="AU2" s="17"/>
+      <c r="AV2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="AW2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY2" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ2" s="16" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1131,191 +1260,275 @@
       <c r="H3" s="7">
         <v>67</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="27">
+        <v>71</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="9">
-        <f t="shared" ref="J3:J11" si="1">J$1</f>
+      <c r="K3" s="9">
+        <f t="shared" ref="K3:K11" si="1">K$1</f>
         <v>2016</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>65</v>
       </c>
-      <c r="M3" s="7">
+      <c r="N3" s="7">
         <v>67</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="27">
+        <v>71</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="9">
-        <f t="shared" ref="O3:O11" si="2">O$1</f>
+      <c r="Q3" s="9">
+        <f t="shared" ref="Q3:Q11" si="2">Q$1</f>
         <v>2017</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="S3" s="7">
         <v>80</v>
       </c>
-      <c r="R3" s="7">
+      <c r="T3" s="7">
         <v>82</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="U3" s="27">
+        <v>86</v>
+      </c>
+      <c r="V3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="9">
-        <f t="shared" ref="T3:T11" si="3">T$1</f>
+      <c r="W3" s="9">
+        <f t="shared" ref="W3:W11" si="3">W$1</f>
         <v>2018</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="7">
+      <c r="Y3" s="7">
         <v>80</v>
       </c>
-      <c r="W3" s="7">
+      <c r="Z3" s="7">
         <v>82</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="AA3" s="27">
+        <v>86</v>
+      </c>
+      <c r="AB3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y3" s="9" t="str">
-        <f t="shared" ref="Y3:Y11" si="4">Y$1</f>
+      <c r="AC3" s="9" t="str">
+        <f t="shared" ref="AC3:AC11" si="4">AC$1</f>
         <v>1/2018</v>
       </c>
-      <c r="Z3" s="18" t="s">
+      <c r="AD3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="9" t="str">
-        <f t="shared" ref="AD3:AD11" si="5">AD$1</f>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI3" s="9" t="str">
+        <f t="shared" ref="AI3:AI11" si="5">AI$1</f>
         <v>2/2018</v>
       </c>
-      <c r="AE3" s="18" t="s">
+      <c r="AJ3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="AF3" s="7">
+      <c r="AK3" s="7">
         <v>18</v>
       </c>
-      <c r="AG3" s="7">
+      <c r="AL3" s="7">
         <v>20</v>
       </c>
-      <c r="AH3" s="19" t="s">
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AI3" s="9" t="str">
-        <f t="shared" ref="AI3:AI11" si="6">AI$1</f>
+      <c r="AO3" s="9" t="str">
+        <f t="shared" ref="AO3:AO11" si="6">AO$1</f>
         <v>3/2018</v>
       </c>
-      <c r="AJ3" s="18" t="s">
+      <c r="AP3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="AK3" s="7">
+      <c r="AQ3" s="7">
         <v>20</v>
       </c>
-      <c r="AL3" s="7">
+      <c r="AR3" s="7">
         <v>22</v>
       </c>
-      <c r="AM3" s="19" t="s">
+      <c r="AS3" s="27"/>
+      <c r="AT3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="AN3" s="9" t="str">
-        <f t="shared" ref="AN3:AN11" si="7">AN$1</f>
+      <c r="AU3" s="9" t="str">
+        <f t="shared" ref="AU3:AU11" si="7">AU$1</f>
         <v>4/2018</v>
       </c>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="7"/>
-      <c r="AQ3" s="7"/>
-      <c r="AR3" s="8"/>
+      <c r="AV3" s="6"/>
+      <c r="AW3" s="7"/>
+      <c r="AX3" s="7"/>
+      <c r="AY3" s="27"/>
+      <c r="AZ3" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="1">
+        <v>1054</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>4</v>
+      </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5">
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1">
+        <v>58</v>
+      </c>
+      <c r="H4" s="1">
+        <v>59</v>
+      </c>
+      <c r="I4" s="28">
+        <v>63</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="5">
+      <c r="L4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="1">
+        <v>58</v>
+      </c>
+      <c r="N4" s="1">
+        <v>59</v>
+      </c>
+      <c r="O4" s="28">
+        <v>63</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="5">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="5">
+      <c r="R4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="1">
+        <v>57</v>
+      </c>
+      <c r="T4" s="1">
+        <v>58</v>
+      </c>
+      <c r="U4" s="28">
+        <v>62</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="W4" s="5">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U4" s="3"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="5" t="str">
+      <c r="X4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>57</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>58</v>
+      </c>
+      <c r="AA4" s="28">
+        <v>62</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="5" t="str">
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI4" s="5" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="5" t="str">
+      <c r="AM4" s="28"/>
+      <c r="AN4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO4" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="28"/>
+      <c r="AT4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU4" s="5" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO4" s="3"/>
-      <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
-      <c r="AR4" s="4"/>
+      <c r="AV4" s="3"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="28"/>
+      <c r="AZ4" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="20">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="23"/>
+      <c r="C5" s="7">
+        <v>288</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" s="9">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -1323,73 +1536,85 @@
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9">
+      <c r="I5" s="27"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="9">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9">
+      <c r="N5" s="7"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="9">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="9">
+      <c r="R5" s="6"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="9">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="9" t="str">
+      <c r="X5" s="6"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="27"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="9" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="9" t="str">
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="9" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="7"/>
       <c r="AL5" s="7"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="9" t="str">
+      <c r="AM5" s="27"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="7"/>
+      <c r="AR5" s="7"/>
+      <c r="AS5" s="27"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="9" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="7"/>
-      <c r="AQ5" s="7"/>
-      <c r="AR5" s="8"/>
+      <c r="AV5" s="6"/>
+      <c r="AW5" s="7"/>
+      <c r="AX5" s="7"/>
+      <c r="AY5" s="27"/>
+      <c r="AZ5" s="8"/>
     </row>
-    <row r="6" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="24"/>
+      <c r="C6" s="1">
+        <v>1212</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -1397,65 +1622,73 @@
       <c r="F6" s="3"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5">
+      <c r="I6" s="28"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K6" s="3"/>
-      <c r="L6" s="1"/>
+      <c r="L6" s="3"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="5">
+      <c r="N6" s="1"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="5">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="5">
+      <c r="R6" s="3"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="5">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U6" s="3"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="5" t="str">
+      <c r="X6" s="3"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="5" t="str">
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="4"/>
+      <c r="AI6" s="5" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="4"/>
-      <c r="AI6" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="1"/>
       <c r="AL6" s="1"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="5" t="str">
+      <c r="AM6" s="28"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="28"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="5" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO6" s="3"/>
-      <c r="AP6" s="1"/>
-      <c r="AQ6" s="1"/>
-      <c r="AR6" s="4"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="1"/>
+      <c r="AY6" s="28"/>
+      <c r="AZ6" s="4"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -1471,65 +1704,73 @@
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9">
+      <c r="I7" s="27"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="9">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9">
+      <c r="N7" s="7"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="9">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="9">
+      <c r="R7" s="6"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="9">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U7" s="6"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="9" t="str">
+      <c r="X7" s="6"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="27"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="9" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="9" t="str">
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="27"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="9" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="7"/>
-      <c r="AG7" s="7"/>
-      <c r="AH7" s="8"/>
-      <c r="AI7" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="7"/>
       <c r="AL7" s="7"/>
-      <c r="AM7" s="8"/>
-      <c r="AN7" s="9" t="str">
+      <c r="AM7" s="27"/>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="27"/>
+      <c r="AT7" s="8"/>
+      <c r="AU7" s="9" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO7" s="6"/>
-      <c r="AP7" s="7"/>
-      <c r="AQ7" s="7"/>
-      <c r="AR7" s="8"/>
+      <c r="AV7" s="6"/>
+      <c r="AW7" s="7"/>
+      <c r="AX7" s="7"/>
+      <c r="AY7" s="27"/>
+      <c r="AZ7" s="8"/>
     </row>
-    <row r="8" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1545,65 +1786,73 @@
       <c r="F8" s="3"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5">
+      <c r="I8" s="28"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="5">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="1"/>
+      <c r="L8" s="3"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="5">
+      <c r="N8" s="1"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="5">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="5">
+      <c r="R8" s="3"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="5">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U8" s="3"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="5" t="str">
+      <c r="X8" s="3"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="4"/>
+      <c r="AC8" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="5" t="str">
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="4"/>
+      <c r="AI8" s="5" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ8" s="3"/>
       <c r="AK8" s="1"/>
       <c r="AL8" s="1"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="5" t="str">
+      <c r="AM8" s="28"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP8" s="3"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="28"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="5" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO8" s="3"/>
-      <c r="AP8" s="1"/>
-      <c r="AQ8" s="1"/>
-      <c r="AR8" s="4"/>
+      <c r="AV8" s="3"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="28"/>
+      <c r="AZ8" s="4"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -1619,65 +1868,73 @@
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9">
+      <c r="I9" s="27"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9">
+      <c r="N9" s="7"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="9">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9">
+      <c r="R9" s="6"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="9">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U9" s="6"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="9" t="str">
+      <c r="X9" s="6"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="27"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="9" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="9" t="str">
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="27"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="9" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE9" s="6"/>
-      <c r="AF9" s="7"/>
-      <c r="AG9" s="7"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="7"/>
       <c r="AL9" s="7"/>
-      <c r="AM9" s="8"/>
-      <c r="AN9" s="9" t="str">
+      <c r="AM9" s="27"/>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="9" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="27"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="9" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO9" s="6"/>
-      <c r="AP9" s="7"/>
-      <c r="AQ9" s="7"/>
-      <c r="AR9" s="8"/>
+      <c r="AV9" s="6"/>
+      <c r="AW9" s="7"/>
+      <c r="AX9" s="7"/>
+      <c r="AY9" s="27"/>
+      <c r="AZ9" s="8"/>
     </row>
-    <row r="10" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1693,65 +1950,73 @@
       <c r="F10" s="3"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5">
+      <c r="I10" s="28"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="5">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="5">
+      <c r="N10" s="1"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="5">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="4"/>
-      <c r="T10" s="5">
+      <c r="R10" s="3"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="5">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U10" s="3"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="5" t="str">
+      <c r="X10" s="3"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="4"/>
+      <c r="AC10" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="4"/>
-      <c r="AD10" s="5" t="str">
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="4"/>
+      <c r="AI10" s="5" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="4"/>
-      <c r="AI10" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="1"/>
       <c r="AL10" s="1"/>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="5" t="str">
+      <c r="AM10" s="28"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP10" s="3"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="28"/>
+      <c r="AT10" s="4"/>
+      <c r="AU10" s="5" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="4"/>
+      <c r="AV10" s="3"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="1"/>
+      <c r="AY10" s="28"/>
+      <c r="AZ10" s="4"/>
     </row>
-    <row r="11" spans="1:44" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -1767,75 +2032,108 @@
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13">
+      <c r="I11" s="29"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="13">
+      <c r="N11" s="11"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="13">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="13">
+      <c r="R11" s="10"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="13">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
-      <c r="U11" s="10"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="13" t="str">
+      <c r="X11" s="10"/>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="11"/>
+      <c r="AA11" s="29"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="13" t="str">
         <f t="shared" si="4"/>
         <v>1/2018</v>
       </c>
-      <c r="Z11" s="10"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="12"/>
-      <c r="AD11" s="13" t="str">
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="11"/>
+      <c r="AF11" s="11"/>
+      <c r="AG11" s="29"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="13" t="str">
         <f t="shared" si="5"/>
         <v>2/2018</v>
-      </c>
-      <c r="AE11" s="10"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="12"/>
-      <c r="AI11" s="13" t="str">
-        <f t="shared" si="6"/>
-        <v>3/2018</v>
       </c>
       <c r="AJ11" s="10"/>
       <c r="AK11" s="11"/>
       <c r="AL11" s="11"/>
-      <c r="AM11" s="12"/>
-      <c r="AN11" s="13" t="str">
+      <c r="AM11" s="29"/>
+      <c r="AN11" s="12"/>
+      <c r="AO11" s="13" t="str">
+        <f t="shared" si="6"/>
+        <v>3/2018</v>
+      </c>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="11"/>
+      <c r="AR11" s="11"/>
+      <c r="AS11" s="29"/>
+      <c r="AT11" s="12"/>
+      <c r="AU11" s="13" t="str">
         <f t="shared" si="7"/>
         <v>4/2018</v>
       </c>
-      <c r="AO11" s="10"/>
-      <c r="AP11" s="11"/>
-      <c r="AQ11" s="11"/>
-      <c r="AR11" s="12"/>
+      <c r="AV11" s="10"/>
+      <c r="AW11" s="11"/>
+      <c r="AX11" s="11"/>
+      <c r="AY11" s="29"/>
+      <c r="AZ11" s="12"/>
+    </row>
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B13" s="42">
+        <f>COUNTA(D3:D11)/A11</f>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+    </row>
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="C14" s="41"/>
+    </row>
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="B15" s="43">
+        <f>A11</f>
+        <v>9</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="40">
+        <f>COUNTA(D3:D11)</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="AI1:AM1"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="Y1:AC1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="AU1:AZ1"/>
+    <mergeCell ref="AO1:AT1"/>
+    <mergeCell ref="AI1:AN1"/>
+    <mergeCell ref="AC1:AH1"/>
+    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="K1:P1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update datatest - 06/08/2019
</commit_message>
<xml_diff>
--- a/fin_scrapy/maya/data/datatest.xlsx
+++ b/fin_scrapy/maya/data/datatest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naama\PycharmProjects\finance_book\fin_scrapy\maya\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6900132C-984A-4A4E-BDF7-DB91863B6DBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962FFAA5-13DA-48E8-A9A8-12F17BBB11C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D9F26097-3032-4D88-B237-30A8AA0DDC42}"/>
   </bookViews>
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>campany</t>
-  </si>
-  <si>
     <t>tckr</t>
   </si>
   <si>
@@ -129,6 +126,12 @@
   </si>
   <si>
     <t>מתוך</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>company</t>
   </si>
 </sst>
 </file>
@@ -640,47 +643,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="13" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="18" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="17" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="13" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="18" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1005,11 +1008,12 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.75" bestFit="1" customWidth="1"/>
     <col min="18" max="23" width="9.33203125" customWidth="1"/>
@@ -1021,217 +1025,225 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="33">
+        <v>2015</v>
+      </c>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="33">
+        <v>2016</v>
+      </c>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="33">
+        <v>2017</v>
+      </c>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="33">
+        <v>2018</v>
+      </c>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="30">
-        <v>2015</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="30">
-        <v>2016</v>
-      </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="30">
-        <v>2017</v>
-      </c>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="30">
-        <v>2018</v>
-      </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="37" t="s">
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="42"/>
+      <c r="AI1" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="34" t="s">
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35"/>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="35"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="34" t="s">
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="38"/>
+      <c r="AS1" s="38"/>
+      <c r="AT1" s="39"/>
+      <c r="AU1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="AP1" s="35"/>
-      <c r="AQ1" s="35"/>
-      <c r="AR1" s="35"/>
-      <c r="AS1" s="35"/>
-      <c r="AT1" s="36"/>
-      <c r="AU1" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV1" s="35"/>
-      <c r="AW1" s="35"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="35"/>
-      <c r="AZ1" s="36"/>
+      <c r="AV1" s="38"/>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="38"/>
+      <c r="AY1" s="38"/>
+      <c r="AZ1" s="39"/>
     </row>
     <row r="2" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="E2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="14" t="s">
+      <c r="H2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="K2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="14" t="s">
+      <c r="O2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="Q2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="14" t="s">
+      <c r="U2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="W2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="W2" s="17"/>
-      <c r="X2" s="14" t="s">
+      <c r="AA2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB2" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="Y2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AA2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="AC2" s="17"/>
       <c r="AD2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH2" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH2" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="AI2" s="17"/>
       <c r="AJ2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN2" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="AK2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN2" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="AO2" s="17"/>
       <c r="AP2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT2" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="AQ2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AR2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AT2" s="16" t="s">
-        <v>13</v>
       </c>
       <c r="AU2" s="17"/>
       <c r="AV2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AX2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AY2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="AZ2" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="AW2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="AX2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="AY2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="AZ2" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.3">
@@ -1239,20 +1251,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="7">
         <v>68</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="9">
         <f t="shared" ref="E3:E11" si="0">E$1</f>
         <v>2015</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7">
         <v>65</v>
@@ -1264,14 +1276,14 @@
         <v>71</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ref="K3:K11" si="1">K$1</f>
         <v>2016</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M3" s="7">
         <v>65</v>
@@ -1283,14 +1295,14 @@
         <v>71</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="9">
         <f t="shared" ref="Q3:Q11" si="2">Q$1</f>
         <v>2017</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S3" s="7">
         <v>80</v>
@@ -1302,14 +1314,14 @@
         <v>86</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="W3" s="9">
         <f t="shared" ref="W3:W11" si="3">W$1</f>
         <v>2018</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Y3" s="7">
         <v>80</v>
@@ -1321,27 +1333,27 @@
         <v>86</v>
       </c>
       <c r="AB3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC3" s="9" t="str">
         <f t="shared" ref="AC3:AC11" si="4">AC$1</f>
         <v>1/2018</v>
       </c>
       <c r="AD3" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AE3" s="7"/>
       <c r="AF3" s="7"/>
       <c r="AG3" s="27"/>
       <c r="AH3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AI3" s="9" t="str">
         <f t="shared" ref="AI3:AI11" si="5">AI$1</f>
         <v>2/2018</v>
       </c>
       <c r="AJ3" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AK3" s="7">
         <v>18</v>
@@ -1351,14 +1363,14 @@
       </c>
       <c r="AM3" s="27"/>
       <c r="AN3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AO3" s="9" t="str">
         <f t="shared" ref="AO3:AO11" si="6">AO$1</f>
         <v>3/2018</v>
       </c>
       <c r="AP3" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AQ3" s="7">
         <v>20</v>
@@ -1368,7 +1380,7 @@
       </c>
       <c r="AS3" s="27"/>
       <c r="AT3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AU3" s="9" t="str">
         <f t="shared" ref="AU3:AU11" si="7">AU$1</f>
@@ -1379,7 +1391,7 @@
       <c r="AX3" s="7"/>
       <c r="AY3" s="27"/>
       <c r="AZ3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:52" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1387,20 +1399,20 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>1054</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
         <v>2015</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1">
         <v>58</v>
@@ -1412,14 +1424,14 @@
         <v>63</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="1"/>
         <v>2016</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4" s="1">
         <v>58</v>
@@ -1431,14 +1443,14 @@
         <v>63</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="5">
         <f t="shared" si="2"/>
         <v>2017</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S4" s="1">
         <v>57</v>
@@ -1450,14 +1462,14 @@
         <v>62</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="W4" s="5">
         <f t="shared" si="3"/>
         <v>2018</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="1">
         <v>57</v>
@@ -1469,7 +1481,7 @@
         <v>62</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AC4" s="5" t="str">
         <f t="shared" si="4"/>
@@ -1480,7 +1492,7 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="28"/>
       <c r="AH4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AI4" s="5" t="str">
         <f t="shared" si="5"/>
@@ -1491,7 +1503,7 @@
       <c r="AL4" s="1"/>
       <c r="AM4" s="28"/>
       <c r="AN4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AO4" s="5" t="str">
         <f t="shared" si="6"/>
@@ -1502,7 +1514,7 @@
       <c r="AR4" s="1"/>
       <c r="AS4" s="28"/>
       <c r="AT4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AU4" s="5" t="str">
         <f t="shared" si="7"/>
@@ -1513,7 +1525,7 @@
       <c r="AX4" s="1"/>
       <c r="AY4" s="28"/>
       <c r="AZ4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
@@ -1521,13 +1533,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="7">
         <v>288</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="0"/>
@@ -1607,13 +1619,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>1212</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
+      <c r="D6" s="24" t="s">
+        <v>5</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
@@ -1693,7 +1705,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="23"/>
@@ -1775,7 +1787,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="24"/>
@@ -1857,7 +1869,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="23"/>
@@ -1939,7 +1951,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="24"/>
@@ -2021,7 +2033,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="25"/>
@@ -2099,25 +2111,25 @@
       <c r="AZ11" s="12"/>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B13" s="42">
+      <c r="B13" s="32">
         <f>COUNTA(D3:D11)/A11</f>
         <v>0.44444444444444442</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="C14" s="41"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B15" s="43">
+      <c r="B15" s="31">
         <f>A11</f>
         <v>9</v>
       </c>
-      <c r="C15" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="40">
+      <c r="C15" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="43">
         <f>COUNTA(D3:D11)</f>
         <v>4</v>
       </c>

</xml_diff>